<commit_message>
finished IOTAII, updated spreadsheet and keeping track of progress w/ feedback
</commit_message>
<xml_diff>
--- a/Sameer's Leetcode Progress.xlsx
+++ b/Sameer's Leetcode Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sameer\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8B7B54-7B6F-40A4-8CC4-B27395E6DB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5E36F1-47AF-43DD-BD16-71435C83A11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{33B1EFDB-2811-48D9-9506-EF5CD89F6C3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="135">
   <si>
     <t>Leetcode Problems Finished</t>
   </si>
@@ -426,6 +426,21 @@
   </si>
   <si>
     <t>Same as usual 2 pointers approach, except you will be comparing lptr and rptr, and always get the maxArea, then you can eventually find the largest area while l &lt; r</t>
+  </si>
+  <si>
+    <t>Find Common Characters</t>
+  </si>
+  <si>
+    <t>This one wont be marked as completed until we can do it 100% by ourselves tomorrow</t>
+  </si>
+  <si>
+    <t>Intersection of 2 Arrays II</t>
+  </si>
+  <si>
+    <t>This one was done well, not sure why we cant shorten the algorithm though, to just check if nums2[j] is in the dict and is valid</t>
+  </si>
+  <si>
+    <t>Initialize count vector for one str, cmp it to second string, add results if there is connection in between, could also make 2 count vectors and just AND them together, considering that diff values could be possible</t>
   </si>
 </sst>
 </file>
@@ -843,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73DF0B43-5C1C-41E1-B4B4-D5EAF7B308E4}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,7 +885,7 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>COUNTA(A4:A1048576)</f>
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1953,6 +1968,49 @@
       </c>
       <c r="I45" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>130</v>
+      </c>
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>132</v>
+      </c>
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" t="s">
+        <v>133</v>
+      </c>
+      <c r="F47" s="1">
+        <v>45532</v>
+      </c>
+      <c r="G47" t="s">
+        <v>41</v>
+      </c>
+      <c r="I47" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>